<commit_message>
add new arr + string
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tranm\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a9c2175c937ce693/Documents/Eclipse/onThiSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB1D8B-E91E-4765-9E88-9F350908B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{40FB1D8B-E91E-4765-9E88-9F350908B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A53FEB-8FCA-467A-985C-EDBB8F7EC7B9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D239FB3-6C3A-4EF9-BAD3-18949551E2F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8D239FB3-6C3A-4EF9-BAD3-18949551E2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
   <si>
     <t>2,2</t>
   </si>
@@ -439,6 +441,39 @@
   <si>
     <t xml:space="preserve">mảng sx: 1 3 4 5 7 </t>
   </si>
+  <si>
+    <t>1(3,1)</t>
+  </si>
+  <si>
+    <t>1(2,0)</t>
+  </si>
+  <si>
+    <t>23 + 47 = machula</t>
+  </si>
+  <si>
+    <t>vi tri= 4</t>
+  </si>
+  <si>
+    <t>3247 + 5machula2 = 3749</t>
+  </si>
+  <si>
+    <t>vi tri= 2</t>
+  </si>
+  <si>
+    <t>machula13 + 75425 = 77038</t>
+  </si>
+  <si>
+    <t>vi tri= 0</t>
+  </si>
+  <si>
+    <t>nếu chỉ tìm chuỗi a có b không thì dùng equal</t>
+  </si>
+  <si>
+    <t>còn nếu chuỗi bất kì có trong b không như ví dụ trên thì dùng contains</t>
+  </si>
+  <si>
+    <t>split dùng để tách chuỗi khi gặp ký tự: ví dụ spli(" ")</t>
+  </si>
 </sst>
 </file>
 
@@ -448,7 +483,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -621,6 +656,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -940,20 +979,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9116AF3F-8507-4DE1-9762-DB7DC7AC6F5A}">
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J25" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+    <sheetView topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="20" max="20" width="13.109375" customWidth="1"/>
+    <col min="20" max="20" width="13.09765625" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="25" max="25" width="15.109375" customWidth="1"/>
+    <col min="25" max="25" width="15.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -961,7 +1000,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -976,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1001,7 +1040,7 @@
       <c r="AD3" s="21"/>
       <c r="AE3" s="21"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1013,7 +1052,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1078,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1158,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I7">
         <v>2</v>
       </c>
@@ -1165,7 +1204,7 @@
       </c>
       <c r="AE7" s="18"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I8">
         <v>3</v>
       </c>
@@ -1223,7 +1262,7 @@
       </c>
       <c r="AE8" s="18"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I9">
         <v>4</v>
       </c>
@@ -1271,7 +1310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I10">
         <v>5</v>
       </c>
@@ -1302,7 +1341,7 @@
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I11">
         <v>6</v>
       </c>
@@ -1319,7 +1358,7 @@
       <c r="R11" s="13"/>
       <c r="S11" s="15"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I12">
         <v>7</v>
       </c>
@@ -1335,7 +1374,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1433,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +1453,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1434,7 +1473,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1451,7 +1490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AA18" t="s">
         <v>54</v>
       </c>
@@ -1462,7 +1501,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AA19" t="s">
         <v>45</v>
       </c>
@@ -1473,7 +1512,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="AA20" t="s">
         <v>39</v>
       </c>
@@ -1484,7 +1523,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>27</v>
       </c>
@@ -1502,7 +1541,7 @@
       </c>
       <c r="Y22" s="19"/>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>31</v>
       </c>
@@ -1533,7 +1572,7 @@
       </c>
       <c r="Y23" s="19"/>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>32</v>
       </c>
@@ -1550,7 +1589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>84</v>
       </c>
@@ -1558,7 +1597,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J30" s="5"/>
       <c r="K30" s="5">
         <v>0</v>
@@ -1573,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J31" s="5">
         <v>0</v>
       </c>
@@ -1594,7 +1633,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="J32" s="5">
         <v>1</v>
       </c>
@@ -1609,7 +1648,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J33" s="5">
         <v>2</v>
       </c>
@@ -1624,7 +1663,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J34" s="5">
         <v>3</v>
       </c>
@@ -1642,7 +1681,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J35" s="5">
         <v>4</v>
       </c>
@@ -1659,7 +1698,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:27" x14ac:dyDescent="0.25">
       <c r="X36" t="s">
         <v>105</v>
       </c>
@@ -1667,12 +1706,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="10:27" x14ac:dyDescent="0.25">
       <c r="P37" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>96</v>
       </c>
@@ -1680,7 +1719,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>95</v>
       </c>
@@ -1688,7 +1727,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>97</v>
       </c>
@@ -1696,7 +1735,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>98</v>
       </c>
@@ -1707,7 +1746,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>99</v>
       </c>
@@ -1715,13 +1754,123 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="10:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="10:27" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
         <v>100</v>
       </c>
       <c r="X43" t="s">
         <v>112</v>
       </c>
+    </row>
+    <row r="45" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>2</v>
+      </c>
+      <c r="V45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+    </row>
+    <row r="47" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+    </row>
+    <row r="48" spans="10:27" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>2</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>3</v>
+      </c>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+    </row>
+    <row r="54" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>2</v>
+      </c>
+      <c r="P54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>2</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="12:22" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>3</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1730,4 +1879,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A2169F-1FE8-43A8-B34D-1AAA93A8E654}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test bài quản lý mảng và bài giao hành nhanh(GHN)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a9c2175c937ce693/Documents/Eclipse/onThiSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{40FB1D8B-E91E-4765-9E88-9F350908B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A53FEB-8FCA-467A-985C-EDBB8F7EC7B9}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{40FB1D8B-E91E-4765-9E88-9F350908B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0822EFB-771E-4D02-8725-344CE52CA17B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8D239FB3-6C3A-4EF9-BAD3-18949551E2F8}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{8D239FB3-6C3A-4EF9-BAD3-18949551E2F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -658,8 +658,53 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>92029</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160414</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A27BC2-866C-B498-4E2E-DF33F6EF61AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6797629" cy="4541914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1885,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A2169F-1FE8-43A8-B34D-1AAA93A8E654}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1939,4 +1984,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF57577-D0DD-4E12-9F4D-889DAB9A71EE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>